<commit_message>
added anon id and removed auto email sending
</commit_message>
<xml_diff>
--- a/temp/TaskBalances.xlsx
+++ b/temp/TaskBalances.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,24 +373,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2</v>
+        <v>11111111</v>
       </c>
       <c r="B2">
-        <v>1235</v>
+        <v>123</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>10809788</v>
+        <v>11111111</v>
       </c>
       <c r="B3">
-        <v>1235</v>
+        <v>125</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>22222222</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>